<commit_message>
removing restriction on dhw types
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/HVAC.xlsx
+++ b/cea/databases/CH/assemblies/HVAC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.santos\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\assemblies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zshi/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/assemblies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37187EA0-C819-4801-A6A7-C1B85C10D85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FE9A55-E5FD-D44F-9FF9-29725E40A400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="4380" windowWidth="23700" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HOT_WATER" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
   <si>
     <t>Description</t>
   </si>
@@ -300,6 +300,18 @@
   </si>
   <si>
     <t>reference</t>
+  </si>
+  <si>
+    <t>HIGH_TEMP</t>
+  </si>
+  <si>
+    <t>LOW_TEMP</t>
+  </si>
+  <si>
+    <t>MEDIUM_TEMP</t>
+  </si>
+  <si>
+    <t>class_dhw</t>
   </si>
 </sst>
 </file>
@@ -393,16 +405,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -698,21 +707,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,84 +730,103 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="5">
         <v>60</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="5">
         <v>45</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="6">
-        <v>35</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="5">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3">
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="5">
         <v>60</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -806,24 +835,24 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" customWidth="1"/>
-    <col min="2" max="3" width="19.81640625" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" customWidth="1"/>
-    <col min="7" max="7" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.81640625" customWidth="1"/>
-    <col min="10" max="10" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,223 +896,223 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="8">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
         <v>500</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.15</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="3">
         <v>90</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>500</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>-0.1</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="4">
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="3">
         <v>70</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>500</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>40</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>20</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>36</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>40</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>20</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>36</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>0.5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>150</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>-0.9</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="4">
+      <c r="G6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="3">
         <v>40</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1097,29 +1126,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.453125" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1166,193 +1195,193 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="8">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>500</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.5</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="3">
         <v>18</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>150</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.7</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3">
         <v>7.5</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>7</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>16</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>500</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0.5</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>7.5</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>7</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>16</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>7.5</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>7</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>16</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="M5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="E6" s="3">
@@ -1386,47 +1415,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>0.1</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>100</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>0.5</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="4">
+      <c r="G7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="3">
         <v>18</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1444,18 +1473,18 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1478,11 +1507,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="2" t="b">
@@ -1501,11 +1530,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C3" s="2" t="b">
@@ -1524,11 +1553,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="2" t="b">
@@ -1547,11 +1576,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="2" t="b">
@@ -1583,13 +1612,13 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.7265625" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1603,11 +1632,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="3">
@@ -1617,11 +1646,11 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="3">
@@ -1631,11 +1660,11 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C4" s="3">
@@ -1645,11 +1674,11 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="3">
@@ -1659,11 +1688,11 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="3">

</xml_diff>